<commit_message>
adding sum of emissions
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BG44"/>
+  <dimension ref="A1:BT44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -724,6 +724,71 @@
           <t>stage5_Al2O3</t>
         </is>
       </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>single_sum_CO2</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>single_sum_H2O</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>single_sum_N2</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>single_sum_O2</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>single_sum_HCl</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>single_sum_Al2O3</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>launchrate</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>total_sum_CO2</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>total_sum_H2O</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>total_sum_N2</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>total_sum_O2</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>total_sum_HCl</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>total_sum_Al2O3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -913,6 +978,45 @@
         <v>0</v>
       </c>
       <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>619785.2085295001</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>251286.7959935</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>7691.081881999999</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>619785.2085295001</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>251286.7959935</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>7691.081881999999</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1102,6 +1206,45 @@
       <c r="BG3" t="n">
         <v>0</v>
       </c>
+      <c r="BH3" t="n">
+        <v>203931</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>81572.39999999999</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>407862</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>163144.8</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -1291,6 +1434,45 @@
       <c r="BG4" t="n">
         <v>0</v>
       </c>
+      <c r="BH4" t="n">
+        <v>92565.75672</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>390875.070437225</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>3361.608</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>56377.60320000001</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>51391.43736</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>86159.60424</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>3</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>277697.27016</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>1172625.211311675</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>10084.824</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>169132.8096</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>154174.31208</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>258478.81272</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1478,6 +1660,45 @@
       <c r="BG5" t="n">
         <v>0</v>
       </c>
+      <c r="BH5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1665,6 +1886,45 @@
       <c r="BG6" t="n">
         <v>0</v>
       </c>
+      <c r="BH6" t="n">
+        <v>255679.2</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>148804.987021973</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO6" t="n">
+        <v>511358.4</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>297609.974043946</v>
+      </c>
+      <c r="BQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1854,6 +2114,45 @@
       <c r="BG7" t="n">
         <v>0</v>
       </c>
+      <c r="BH7" t="n">
+        <v>539804.6476216</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>236616.541725573</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>539804.6476216</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>236616.541725573</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2043,6 +2342,45 @@
       <c r="BG8" t="n">
         <v>0</v>
       </c>
+      <c r="BH8" t="n">
+        <v>965992.819054</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>368333.873780973</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO8" t="n">
+        <v>1931985.638108</v>
+      </c>
+      <c r="BP8" t="n">
+        <v>736667.747561946</v>
+      </c>
+      <c r="BQ8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -2230,6 +2568,45 @@
       <c r="BG9" t="n">
         <v>0</v>
       </c>
+      <c r="BH9" t="n">
+        <v>93065.48559973601</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>76192.675747448</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>88858.564929056</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>3</v>
+      </c>
+      <c r="BO9" t="n">
+        <v>279196.4567992081</v>
+      </c>
+      <c r="BP9" t="n">
+        <v>228578.027242344</v>
+      </c>
+      <c r="BQ9" t="n">
+        <v>266575.694787168</v>
+      </c>
+      <c r="BR9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -2419,6 +2796,45 @@
       <c r="BG10" t="n">
         <v>0</v>
       </c>
+      <c r="BH10" t="n">
+        <v>88305.58965048601</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>72295.750842198</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>84313.834726056</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN10" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO10" t="n">
+        <v>176611.179300972</v>
+      </c>
+      <c r="BP10" t="n">
+        <v>144591.501684396</v>
+      </c>
+      <c r="BQ10" t="n">
+        <v>168627.669452112</v>
+      </c>
+      <c r="BR10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -2606,6 +3022,45 @@
       <c r="BG11" t="n">
         <v>0</v>
       </c>
+      <c r="BH11" t="n">
+        <v>217051.2552858</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>177699.7756794</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>207239.6972568</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>6</v>
+      </c>
+      <c r="BO11" t="n">
+        <v>1302307.5317148</v>
+      </c>
+      <c r="BP11" t="n">
+        <v>1066198.6540764</v>
+      </c>
+      <c r="BQ11" t="n">
+        <v>1243438.1835408</v>
+      </c>
+      <c r="BR11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -2795,6 +3250,45 @@
       <c r="BG12" t="n">
         <v>0</v>
       </c>
+      <c r="BH12" t="n">
+        <v>178037.683502378</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>145759.380102154</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>169989.690134488</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO12" t="n">
+        <v>356075.367004756</v>
+      </c>
+      <c r="BP12" t="n">
+        <v>291518.760204308</v>
+      </c>
+      <c r="BQ12" t="n">
+        <v>339979.380268976</v>
+      </c>
+      <c r="BR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -2986,6 +3480,45 @@
       <c r="BG13" t="n">
         <v>0</v>
       </c>
+      <c r="BH13" t="n">
+        <v>155398.153784376</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>154329.364946355</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>148373.554910496</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN13" t="n">
+        <v>11</v>
+      </c>
+      <c r="BO13" t="n">
+        <v>1709379.691628136</v>
+      </c>
+      <c r="BP13" t="n">
+        <v>1697623.014409905</v>
+      </c>
+      <c r="BQ13" t="n">
+        <v>1632109.104015456</v>
+      </c>
+      <c r="BR13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -3177,6 +3710,45 @@
       <c r="BG14" t="n">
         <v>0</v>
       </c>
+      <c r="BH14" t="n">
+        <v>155398.153784376</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>154329.364946355</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>148373.554910496</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN14" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO14" t="n">
+        <v>155398.153784376</v>
+      </c>
+      <c r="BP14" t="n">
+        <v>154329.364946355</v>
+      </c>
+      <c r="BQ14" t="n">
+        <v>148373.554910496</v>
+      </c>
+      <c r="BR14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -3366,6 +3938,45 @@
       <c r="BG15" t="n">
         <v>0</v>
       </c>
+      <c r="BH15" t="n">
+        <v>123610.8363436</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>101200.1421548</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>118023.1474256</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN15" t="n">
+        <v>5</v>
+      </c>
+      <c r="BO15" t="n">
+        <v>618054.181718</v>
+      </c>
+      <c r="BP15" t="n">
+        <v>506000.710774</v>
+      </c>
+      <c r="BQ15" t="n">
+        <v>590115.737128</v>
+      </c>
+      <c r="BR15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS15" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -3555,6 +4166,45 @@
       <c r="BG16" t="n">
         <v>0</v>
       </c>
+      <c r="BH16" t="n">
+        <v>123610.8363436</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>101200.1421548</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>118023.1474256</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN16" t="n">
+        <v>9</v>
+      </c>
+      <c r="BO16" t="n">
+        <v>1112497.5270924</v>
+      </c>
+      <c r="BP16" t="n">
+        <v>910801.2793932001</v>
+      </c>
+      <c r="BQ16" t="n">
+        <v>1062208.3268304</v>
+      </c>
+      <c r="BR16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -3742,6 +4392,45 @@
       <c r="BG17" t="n">
         <v>0</v>
       </c>
+      <c r="BH17" t="n">
+        <v>459726.75</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>403500.741628186</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN17" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO17" t="n">
+        <v>459726.75</v>
+      </c>
+      <c r="BP17" t="n">
+        <v>403500.741628186</v>
+      </c>
+      <c r="BQ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -3931,6 +4620,45 @@
       <c r="BG18" t="n">
         <v>0</v>
       </c>
+      <c r="BH18" t="n">
+        <v>79548.14588077</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>32634.84157661</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>1859.84343692</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN18" t="n">
+        <v>4</v>
+      </c>
+      <c r="BO18" t="n">
+        <v>318192.58352308</v>
+      </c>
+      <c r="BP18" t="n">
+        <v>130539.36630644</v>
+      </c>
+      <c r="BQ18" t="n">
+        <v>7439.37374768</v>
+      </c>
+      <c r="BR18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS18" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -4120,6 +4848,45 @@
       <c r="BG19" t="n">
         <v>0</v>
       </c>
+      <c r="BH19" t="n">
+        <v>1162047.6</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>464819.04</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN19" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO19" t="n">
+        <v>2324095.2</v>
+      </c>
+      <c r="BP19" t="n">
+        <v>929638.0800000001</v>
+      </c>
+      <c r="BQ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -4311,6 +5078,45 @@
       <c r="BG20" t="n">
         <v>0</v>
       </c>
+      <c r="BH20" t="n">
+        <v>1162047.6</v>
+      </c>
+      <c r="BI20" t="n">
+        <v>491923.998747387</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN20" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO20" t="n">
+        <v>2324095.2</v>
+      </c>
+      <c r="BP20" t="n">
+        <v>983847.9974947741</v>
+      </c>
+      <c r="BQ20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -4500,6 +5306,45 @@
       <c r="BG21" t="n">
         <v>0</v>
       </c>
+      <c r="BH21" t="n">
+        <v>21420</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>526556.004917918</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN21" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO21" t="n">
+        <v>21420</v>
+      </c>
+      <c r="BP21" t="n">
+        <v>526556.004917918</v>
+      </c>
+      <c r="BQ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -4689,6 +5534,45 @@
       <c r="BG22" t="n">
         <v>0</v>
       </c>
+      <c r="BH22" t="n">
+        <v>35595</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>14238</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN22" t="n">
+        <v>6</v>
+      </c>
+      <c r="BO22" t="n">
+        <v>213570</v>
+      </c>
+      <c r="BP22" t="n">
+        <v>85428</v>
+      </c>
+      <c r="BQ22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -4880,6 +5764,45 @@
       <c r="BG23" t="n">
         <v>0</v>
       </c>
+      <c r="BH23" t="n">
+        <v>269340.6392612</v>
+      </c>
+      <c r="BI23" t="n">
+        <v>83405.208554275</v>
+      </c>
+      <c r="BJ23" t="n">
+        <v>190.135249825</v>
+      </c>
+      <c r="BK23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN23" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO23" t="n">
+        <v>269340.6392612</v>
+      </c>
+      <c r="BP23" t="n">
+        <v>83405.208554275</v>
+      </c>
+      <c r="BQ23" t="n">
+        <v>190.135249825</v>
+      </c>
+      <c r="BR23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -5067,6 +5990,45 @@
       <c r="BG24" t="n">
         <v>0</v>
       </c>
+      <c r="BH24" t="n">
+        <v>626125.5</v>
+      </c>
+      <c r="BI24" t="n">
+        <v>250450.2</v>
+      </c>
+      <c r="BJ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN24" t="n">
+        <v>31</v>
+      </c>
+      <c r="BO24" t="n">
+        <v>19409890.5</v>
+      </c>
+      <c r="BP24" t="n">
+        <v>7763956.2</v>
+      </c>
+      <c r="BQ24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -5254,6 +6216,45 @@
       <c r="BG25" t="n">
         <v>0</v>
       </c>
+      <c r="BH25" t="n">
+        <v>154337.4</v>
+      </c>
+      <c r="BI25" t="n">
+        <v>61734.96000000001</v>
+      </c>
+      <c r="BJ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN25" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO25" t="n">
+        <v>154337.4</v>
+      </c>
+      <c r="BP25" t="n">
+        <v>61734.96000000001</v>
+      </c>
+      <c r="BQ25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS25" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -5445,6 +6446,45 @@
       <c r="BG26" t="n">
         <v>0</v>
       </c>
+      <c r="BH26" t="n">
+        <v>558207.8130101881</v>
+      </c>
+      <c r="BI26" t="n">
+        <v>345375.799107644</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>108866.564850448</v>
+      </c>
+      <c r="BK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN26" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO26" t="n">
+        <v>558207.8130101881</v>
+      </c>
+      <c r="BP26" t="n">
+        <v>345375.799107644</v>
+      </c>
+      <c r="BQ26" t="n">
+        <v>108866.564850448</v>
+      </c>
+      <c r="BR26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -5626,6 +6666,45 @@
       <c r="BG27" t="n">
         <v>0</v>
       </c>
+      <c r="BH27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -5815,6 +6894,45 @@
       <c r="BG28" t="n">
         <v>0</v>
       </c>
+      <c r="BH28" t="n">
+        <v>853661.9783743999</v>
+      </c>
+      <c r="BI28" t="n">
+        <v>419330.281121</v>
+      </c>
+      <c r="BJ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN28" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO28" t="n">
+        <v>853661.9783743999</v>
+      </c>
+      <c r="BP28" t="n">
+        <v>419330.281121</v>
+      </c>
+      <c r="BQ28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS28" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -6004,6 +7122,45 @@
       <c r="BG29" t="n">
         <v>0</v>
       </c>
+      <c r="BH29" t="n">
+        <v>426830.9891872</v>
+      </c>
+      <c r="BI29" t="n">
+        <v>287414.2803898</v>
+      </c>
+      <c r="BJ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN29" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO29" t="n">
+        <v>426830.9891872</v>
+      </c>
+      <c r="BP29" t="n">
+        <v>287414.2803898</v>
+      </c>
+      <c r="BQ29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -6185,6 +7342,45 @@
       <c r="BG30" t="n">
         <v>0</v>
       </c>
+      <c r="BH30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN30" t="n">
+        <v>4</v>
+      </c>
+      <c r="BO30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -6370,6 +7566,45 @@
       <c r="BG31" t="n">
         <v>0</v>
       </c>
+      <c r="BH31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN31" t="n">
+        <v>2</v>
+      </c>
+      <c r="BO31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -6561,6 +7796,45 @@
       <c r="BG32" t="n">
         <v>0</v>
       </c>
+      <c r="BH32" t="n">
+        <v>69771.439105992</v>
+      </c>
+      <c r="BI32" t="n">
+        <v>21563.498071332</v>
+      </c>
+      <c r="BJ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN32" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO32" t="n">
+        <v>69771.439105992</v>
+      </c>
+      <c r="BP32" t="n">
+        <v>21563.498071332</v>
+      </c>
+      <c r="BQ32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -6748,6 +8022,45 @@
       <c r="BG33" t="n">
         <v>0</v>
       </c>
+      <c r="BH33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN33" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS33" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -6937,6 +8250,45 @@
       <c r="BG34" t="n">
         <v>0</v>
       </c>
+      <c r="BH34" t="n">
+        <v>63397.90106715</v>
+      </c>
+      <c r="BI34" t="n">
+        <v>19593.698150775</v>
+      </c>
+      <c r="BJ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO34" t="n">
+        <v>63397.90106715</v>
+      </c>
+      <c r="BP34" t="n">
+        <v>19593.698150775</v>
+      </c>
+      <c r="BQ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -7126,6 +8478,45 @@
       <c r="BG35" t="n">
         <v>0</v>
       </c>
+      <c r="BH35" t="n">
+        <v>273061.1840394</v>
+      </c>
+      <c r="BI35" t="n">
+        <v>203962.607316717</v>
+      </c>
+      <c r="BJ35" t="n">
+        <v>224011.849273656</v>
+      </c>
+      <c r="BK35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN35" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO35" t="n">
+        <v>273061.1840394</v>
+      </c>
+      <c r="BP35" t="n">
+        <v>203962.607316717</v>
+      </c>
+      <c r="BQ35" t="n">
+        <v>224011.849273656</v>
+      </c>
+      <c r="BR35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -7317,6 +8708,45 @@
       <c r="BG36" t="n">
         <v>0</v>
       </c>
+      <c r="BH36" t="n">
+        <v>281116.3925689</v>
+      </c>
+      <c r="BI36" t="n">
+        <v>210557.403310217</v>
+      </c>
+      <c r="BJ36" t="n">
+        <v>231702.931155656</v>
+      </c>
+      <c r="BK36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN36" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO36" t="n">
+        <v>281116.3925689</v>
+      </c>
+      <c r="BP36" t="n">
+        <v>210557.403310217</v>
+      </c>
+      <c r="BQ36" t="n">
+        <v>231702.931155656</v>
+      </c>
+      <c r="BR36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -7510,6 +8940,45 @@
       <c r="BG37" t="n">
         <v>0</v>
       </c>
+      <c r="BH37" t="n">
+        <v>287536.02897828</v>
+      </c>
+      <c r="BI37" t="n">
+        <v>235960.8895412</v>
+      </c>
+      <c r="BJ37" t="n">
+        <v>277128.53075764</v>
+      </c>
+      <c r="BK37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN37" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO37" t="n">
+        <v>287536.02897828</v>
+      </c>
+      <c r="BP37" t="n">
+        <v>235960.8895412</v>
+      </c>
+      <c r="BQ37" t="n">
+        <v>277128.53075764</v>
+      </c>
+      <c r="BR37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -7691,6 +9160,45 @@
       <c r="BG38" t="n">
         <v>0</v>
       </c>
+      <c r="BH38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -7876,6 +9384,45 @@
       <c r="BG39" t="n">
         <v>0</v>
       </c>
+      <c r="BH39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN39" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS39" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -8065,6 +9612,45 @@
       <c r="BG40" t="n">
         <v>0</v>
       </c>
+      <c r="BH40" t="n">
+        <v>245070</v>
+      </c>
+      <c r="BI40" t="n">
+        <v>98028</v>
+      </c>
+      <c r="BJ40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN40" t="n">
+        <v>8</v>
+      </c>
+      <c r="BO40" t="n">
+        <v>1960560</v>
+      </c>
+      <c r="BP40" t="n">
+        <v>784224</v>
+      </c>
+      <c r="BQ40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -8254,6 +9840,45 @@
       <c r="BG41" t="n">
         <v>0</v>
       </c>
+      <c r="BH41" t="n">
+        <v>245070</v>
+      </c>
+      <c r="BI41" t="n">
+        <v>98028</v>
+      </c>
+      <c r="BJ41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN41" t="n">
+        <v>13</v>
+      </c>
+      <c r="BO41" t="n">
+        <v>3185910</v>
+      </c>
+      <c r="BP41" t="n">
+        <v>1274364</v>
+      </c>
+      <c r="BQ41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS41" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -8439,6 +10064,45 @@
       <c r="BG42" t="n">
         <v>0</v>
       </c>
+      <c r="BH42" t="n">
+        <v>157815</v>
+      </c>
+      <c r="BI42" t="n">
+        <v>63126</v>
+      </c>
+      <c r="BJ42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS42" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -8630,6 +10294,45 @@
       <c r="BG43" t="n">
         <v>0</v>
       </c>
+      <c r="BH43" t="n">
+        <v>249053.66676368</v>
+      </c>
+      <c r="BI43" t="n">
+        <v>101289.42638224</v>
+      </c>
+      <c r="BJ43" t="n">
+        <v>3803.58958528</v>
+      </c>
+      <c r="BK43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN43" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO43" t="n">
+        <v>249053.66676368</v>
+      </c>
+      <c r="BP43" t="n">
+        <v>101289.42638224</v>
+      </c>
+      <c r="BQ43" t="n">
+        <v>3803.58958528</v>
+      </c>
+      <c r="BR43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS43" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -8819,6 +10522,45 @@
         <v>0</v>
       </c>
       <c r="BG44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH44" t="n">
+        <v>392679.331262961</v>
+      </c>
+      <c r="BI44" t="n">
+        <v>121497.713334</v>
+      </c>
+      <c r="BJ44" t="n">
+        <v>255.903269892</v>
+      </c>
+      <c r="BK44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN44" t="n">
+        <v>3</v>
+      </c>
+      <c r="BO44" t="n">
+        <v>1178037.993788883</v>
+      </c>
+      <c r="BP44" t="n">
+        <v>364493.140002</v>
+      </c>
+      <c r="BQ44" t="n">
+        <v>767.709809676</v>
+      </c>
+      <c r="BR44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS44" t="n">
+        <v>0</v>
+      </c>
+      <c r="BT44" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>